<commit_message>
Leerzeichen auf Windows geändert
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Datum</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Sichtfeld: mit TriggerCollider ODER mit Raycasting/Angle?</t>
+  </si>
+  <si>
+    <t>https://gamedev.stackexchange.com/questions/104773/vision-cone-for-enemy-ai-in-unity-2d</t>
+  </si>
+  <si>
+    <t>http://answers.unity3d.com/questions/414479/2d-enemy-field-of-vision-script.html</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rQG9aUWarwE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=mBGUY7EUxXQ</t>
   </si>
 </sst>
 </file>
@@ -440,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +470,7 @@
     <col min="5" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +487,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>42951</v>
       </c>
@@ -489,7 +504,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
@@ -503,12 +518,32 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>42953</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Guards can now be dragged along with the Player
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Datum</t>
   </si>
@@ -81,12 +81,15 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=mBGUY7EUxXQ</t>
+  </si>
+  <si>
+    <t>Wachen können gezogen/geschoben werden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -454,11 +457,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,6 +549,14 @@
         <v>18</v>
       </c>
     </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>42985</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Menues added. Objects somewhat implemented, but not working correctly yet.
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Datum</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Wachen können gezogen/geschoben werden</t>
+  </si>
+  <si>
+    <t>[Objekt aufnehmen/werfen noch mit Bugs]; Menüs eingeführt für Pause/Gewonnen/Verloren</t>
   </si>
 </sst>
 </file>
@@ -458,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,6 +560,14 @@
         <v>19</v>
       </c>
     </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>42986</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pathfinding Package added. Objects can now be thrown.
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Datum</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>[Objekt aufnehmen/werfen noch mit Bugs]; Menüs eingeführt für Start/Pause/Gewonnen/Verloren</t>
+  </si>
+  <si>
+    <t>https://arongranberg.com/astar/download</t>
+  </si>
+  <si>
+    <t>https://ironic.games/unity-asset-store-reviews/unity-navmesh-vs-a-star-pathfinding-vs-apex-path</t>
+  </si>
+  <si>
+    <t>Nav-Mesh: mit Unity nicht in 2D, ohne weiteres</t>
   </si>
 </sst>
 </file>
@@ -461,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,6 +577,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>42986</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Testversion for throwing objects rudimentary added.
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Datum</t>
   </si>
@@ -96,6 +96,48 @@
   </si>
   <si>
     <t>Nav-Mesh: mit Unity nicht in 2D, ohne weiteres</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_08_04.exe</t>
+  </si>
+  <si>
+    <t>Entwicklung</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_08_07.exe</t>
+  </si>
+  <si>
+    <t>Sichtfeld implementiert</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_07.exe</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_08.exe</t>
+  </si>
+  <si>
+    <t>Marcus</t>
+  </si>
+  <si>
+    <t>Wachen sollten sich langsam drehen; Sichtfeld sichtbar kleiner wenn verkleidet; globale Beleuchtung</t>
+  </si>
+  <si>
+    <t>Neue Features</t>
+  </si>
+  <si>
+    <t>Object aufnehmen/werfen: Richtung kann bestimmt werden, Kraft noch konstant; P: über Wände rüber? Schwer in 2D Topdown! Ab wann über Wand/bis wann gegen Wand? Insgesamt deaktivieren?</t>
+  </si>
+  <si>
+    <t>Loslassen von Shift-Taste wird nicht immer korrekt registriert</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_09.exe</t>
   </si>
 </sst>
 </file>
@@ -470,125 +512,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="2" max="2" width="37.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>42951</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>42953</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
+        <v>42954</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>42985</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="B8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="F8" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>42986</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="B9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>42986</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>42987</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Items can be thrown now. Power of throw can be changed. Power Meter displays power level.
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>Datum</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>DiscordiaAgency_Demo_2017_09_09.exe</t>
+  </si>
+  <si>
+    <t>Object wird jetzt nur bis zur nächsten Wand geworfen; Poweranzeige ist implementiert; Sichtradius der Wachen korrekt kleiner, wenn Spieler verkleidet</t>
   </si>
 </sst>
 </file>
@@ -512,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,6 +738,20 @@
         <v>35</v>
       </c>
     </row>
+    <row r="12" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>42988</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
A*-Pathfinding is working. Guards are running to sound of object now. Guards are hunting player now.
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>Datum</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>Object wird jetzt nur bis zur nächsten Wand geworfen; Poweranzeige ist implementiert; Sichtradius der Wachen korrekt kleiner, wenn Spieler verkleidet</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_12.exe</t>
+  </si>
+  <si>
+    <t>A* ist drin; Wachen können patrouillieren, zum Gegenstand laufen, Spieler jagen; Schießen fehlt noch</t>
   </si>
 </sst>
 </file>
@@ -515,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,6 +758,23 @@
         <v>38</v>
       </c>
     </row>
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>42990</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Guards are shooting at Player and chasing him.
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>Datum</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>A* ist drin; Wachen können patrouillieren, zum Gegenstand laufen, Spieler jagen; Schießen fehlt noch</t>
+  </si>
+  <si>
+    <t>Wachen stehen beim erreichten Gegenstand ineinander; Wachen drehen sich noch nicht korrekt zur Wand; Wachen drehen sich noch nicht korrekt zum Spieler; manchmal Absturz, weil sich eine Coroutine aufhängt…? (Wachen patrouillieren &amp; Gegenstand rotieren)</t>
+  </si>
+  <si>
+    <t>Wachen können schießen &amp; Spieler jagen</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_13.exe</t>
   </si>
 </sst>
 </file>
@@ -521,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,6 +784,26 @@
         <v>40</v>
       </c>
     </row>
+    <row r="14" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>42991</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Info-Text at start of level. Guards change colors. Stop at beginning of seeking mode.
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>Datum</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>DiscordiaAgency_Demo_2017_09_13.exe</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_15.exe</t>
+  </si>
+  <si>
+    <t>insg. 6 Level eingebaut; Wachen können stationär sein; "globales" Alarmsystem: Wachen entdecken Leichen &amp; geben größeren Suchradius an alle Wachen weiter</t>
   </si>
 </sst>
 </file>
@@ -530,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,6 +810,34 @@
         <v>41</v>
       </c>
     </row>
+    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>42993</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel-Tabelle mit Testergebnissen aktualisiert
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="59">
   <si>
     <t>Datum</t>
   </si>
@@ -161,7 +161,112 @@
     <t>DiscordiaAgency_Demo_2017_09_15.exe</t>
   </si>
   <si>
-    <t>insg. 6 Level eingebaut; Wachen können stationär sein; "globales" Alarmsystem: Wachen entdecken Leichen &amp; geben größeren Suchradius an alle Wachen weiter</t>
+    <t>DiscordiaAgency_Demo_2017_09_16.exe</t>
+  </si>
+  <si>
+    <t>Sound; Wachen ändern Farben bei Statusänderung; 6. Level schwerer; Ziel erst erreicht, wenn ganz drauf; Level 3: weniger Wand, damit man vorbei kommt; Level 3: Wache weiter links; FOV-Farben geändert (verkleidet ist jetzt gleiche Farbe, nur kleiner); Wachen bleiben jetzt 4 Sekunden beim Geräusch anstatt 3; Wurfobjekt wird größer, dann kleiner (beim Werfen); Wachen reagieren = stoppen sofort, wenn Objekt aufschlägt, nicht erst mit Verzögerung; Level 2: eine Wache stationär, damit man nicht schon Mechanik von Level 3 nutzt</t>
+  </si>
+  <si>
+    <t>Wachen sollten Farbe ändern; Wachen sollten länger nach Geräusch suchen; Wachen sollten sofort auf Geräusch reagieren; Objekt sollte beim Werfen größer und wieder kleiner skalieren; Level 6 zu leicht; man kann auch geschickt den Kugeln ausweichen &amp; trotz Entdeckung gewinnen - das ist gut; Vorschläge zum Erweitern: Achievements</t>
+  </si>
+  <si>
+    <t>insg. 6 Level eingebaut; Wachen können stationär sein; "globales" Alarmsystem: Wachen entdecken Leichen &amp; geben größeren Suchradius an alle Wachen weiter; Geschwindigkeit und Feuerrate von Kugeln angepasst; Wurfgeschwindigkeit angepasst</t>
+  </si>
+  <si>
+    <t>Spring Joint (beim Draggen der Wache) ist zu lose ("Tanzen"); wenn Wachen schon Jagen geht trotzdem noch der Suchmodus an</t>
+  </si>
+  <si>
+    <t>Space für nächstes Level, nicht Enter (ist man gewohnt); Sound für Wachen, wenn sie toten Körper finden?; Sichtradius: seitliches Reinschieben von totem Körper löst nicht immer gleich aus; "Hold Q and release to throw" besser; nicht "Tutorial" nennen, einfach Angry-Bird-mäßig neue Mechaniken einführen und pro Mechanik mehrere Level mit ansteigendem Schwierigkeitsgrad; mehr Level; Sichtradius der Wachen, wenn alerted, ist irgendwie zu groß?</t>
+  </si>
+  <si>
+    <t>Mathias</t>
+  </si>
+  <si>
+    <t>- Nach dem Klick auf Start hängt das Spiel ohne Feedback, bis das
+Level startet. Da war ich mir erst nicht sicher, ob es lädt oder
+abgestürzt ist. Eine Rückmeldung ("wird geladen") wäre schön.
+- Nach Beenden eines Levels, sollte Space zum Weitermachen und Enter
+zum Wiederholen verwendet werden. Space ist ansonsten immer die Taste
+zum Fortsetzen, außer in der Situation. Außerdem kann man bei
+wasd-Steuerung direkt mit dem Daumen drauf hauen und muss nicht die
+Hand zur Enter-Taste bewegen.
+- Bonus: Z und Y sind auf englischen und norwegischen Tastaturen
+vertauscht. Es wäre mega-cool, wenn die Tastenbelegung automatisch
+entsprechend der Tastatur (oder Betriebssystemsprache oder so)
+angepasst werden würde.
+- Ansonsten ist die Bedienung gut erklärt und auch leicht verständlich.
+- Die Bewegung der Spielfigur ist für meinen Geschmack zu langsam.
+Evtl. sollte auch die Bewegungs-Startbeschleunigung erhöht werden
+(Bremsgeschwindigkeit ist ok)
+- Shift loslassen triggert manchmal nicht. D.h. ich zieh einen Gegner
+weiter, obwohl ich Shift losgelassen hab. Nochmal Shift drücken (und
+loslassen) löst das Problem. Ich konnte es leider nicht gezielt
+reproduzieren, es ist mir aber zwei oder drei Mal in einem
+Durchspielen passiert.
+- Die Idee mit dem Stein find ich sehr gut. Auch, wie die Wachen
+reagieren. Allerdings wäre es schön, eine ungefähre Vorstellung davon
+zu bekommen, wie weit die Ablenkung reicht (kommt aber im Spiel vlt.
+auch mit der Erfahrung). Das Drehen des Steins ist mir zu langsam.
+Willst du bei einer reinen Tastaturbedienung bleiben? Ansonsten könnte
+man den Stein mit der Maus zielen und werfen.
+- Speichern zwischen den Leveln wäre schön, aber das kommt sicher eh noch.
+- Nachdem du soviel von Unity und Shadern erzählt hattest, war die
+Grafik dann doch etwas enttäuschend, aber ich versteh schon, dass erst
+der Unterbau laufen muss :)
+- Die Level fand ich nicht zu schwierig, sondern eher zu leicht. Fies
+fand ich Level 6(?), wo eine Wache wegläuft und dann direkt zurück
+kommt und einen erwischt, selbst wenn man sich nicht bewegt hat. Im
+Prinzip fänd ich es besser, wenn man an seinem Startpunkt nicht
+entdeckt werden könnte, sodass man am Anfang in Ruhe die
+Bewegungsmuster der Wachen angucken kann, ohne gleich erschossen zu
+werden. Es kann natürlich mehr Action reinbringen, wenn man auch am
+Anfang erwischt werden kann.
+- Technische Probleme oder Abstürze hatte ich nicht, wobei ich auch
+nicht viel mit Auflösung, Window/Fullscreen usw. rumgespielt hab.</t>
+  </si>
+  <si>
+    <t>Beim Start auf dem Reiter "Input" sieht die Bedienung erstmal recht kompliziert aus mit vielen Tasten, aber das wird ja im Spiel schrittweise erklärt, das verstehe sogar ich früh morgens :o)
+Optisch finde ich das Ziel nicht so passend zum Spiel und den Gegner im Level 1 (evtl. später auch, soweit bin ich noch nicht). Es ist zwar eindeutig, was was ist, aber farblich und von der Form her irgendwie noch nicht so stimmig finde ich.
+Der Level 1-Text spricht davon, daß die Guards mich nicht "sehen" dürfen. Damit ist nicht ganz klar, daß ich mich zwar in ihrer Nähe, aber halt nur nicht direkt vor ihnen befinden darf.
+Nachtrag: Jetzt habe ich den grauen "Sichtkegel" entdeckt. Der ist optisch viel zu schlecht vom hellblauen Hintergrund zu unterscheiden!
+Auch in Level 1 kann ich offensichtlich schon E, F und Shift nutzen, was links als Text angezeigt wird, aber laut einleitendem Text  nicht zu erwarten war. Das würde ich eher schrittweise einführen bzw. hier noch deaktivieren.
+In Level 2 ist mir nicht klar, warum ich einen Guard mitnehmen soll (Shift), das ist ja erst in Level 3 erforderlich. Der Anspruch steigt von Level 1 zu Level 2 relativ stark - evtl. zu stark? Ich hab zumindest einige Versuche gebraucht, um das Verhalten des senkrechten Guards zu verstehen (da hatte ich allerdings auch den Sichtkegel noch nicht entdeckt).
+In Level 3 hab ich den ersten Guard ausgeknockt und dann abgeschleppt, wurde ihn dann aber nicht mehr los, der blieb an mir kleben, auch ohne Shift. Sieht mir nach eine Fehler aus.
+Manchmal bin ich schon nach einem Treffer tot, einige Male hatte ich den Eindruck, daß mehrere Schüsse nötig waren.
+Auch die "verkürzten Sichtkegel" nach Drücken von F sind optisch nicht gut erkennbar. Zumindest nicht an meinem Laptopmonitor.
+Warum gibt es im Ordner Dateien von level0 bis level10, aber ich darf nur bis Level 6 (glaube ich) spielen?? :-)
+Das Spiel macht Spaß! Simple aber trotzdem abwechselungsreich. Vielleicht läßt sich die Lernkurve ja noch etwas abflachen (Level 2 leichter), dann paßt das auch mit dem Anspruch finde ich.
+Als Erweiterung könnte ich mir noch magnetische Objekte vorstellen, die Schüsse ablenken, eine kurzzeitige Unbesiegbarkeit (z.B. auch dadurch, daß besiegte Guards als Schild dienen, wenn man sie mitnimmt) oder die Möglichkeit, mit besiegten Guards z.B. Wände sprengen zu können. Da geht noch was ;-)</t>
+  </si>
+  <si>
+    <t>Lars Neumann</t>
+  </si>
+  <si>
+    <t>Marcus Riemer</t>
+  </si>
+  <si>
+    <t>Erweiterungsvorschläge: mehr Level, bessers Interface, Schalter für Sound (anstatt Stein), Nachtlevel, Beleuchtung</t>
+  </si>
+  <si>
+    <t>-Gute Funktion mit dem ablenken durch das werfen von Steinen, jedoch würde ich es besser finden, wenn die Guards dann nicht alle auf exakt die Selbe Position laufen, sondern maximal in die selber Ecke oder die Blickrichtung ändern.
+- Ich würde einen größeren Kontrast in die Farbwahl bringen. Generell sind viele Blau-Töne vertreten. Eventuell könnte man zum Beispiel realistische Farben nehmen. Beispielsweise Beige für Bürogebäude oder Stahl-Grau für „Agency-Gebäude".
+-Die Wände würde ich nicht nur mit einem Muster Kennzeichen, sondern eher In kompletter unterschiedlicher Farbe machen (hilft dann auch direkt beim Punkto monotone Farbwahl).
+-Die Steuerung wirkt ein wenig schwammig, vor allem mit einer bewusstlosen Wache im Schlepptau ist das genaue manövrieren relativ schwer.
+- Zudem kommt es vor, dass man ne Wache in die Ecke zieht oder einfach an eine Wand und sie einen dann blockiert, obwohl noch genug Platz zum durchkommen wäre.
+-Die Musik ist passend für solch eine Spielart, allerdings fände ich lautstärke-Regelung innerhalb des Games (z.B. in einer Einstellung Funktion) hilfreich.
+-Für diese Anzahl an Leveln ist es auch so angenehm, sollte allerdings das Spiel noch ausgebaut werde und mit mehr Leveln ausgestattet sein, dann wäre zumindest eine kleine Abwandlung der verwendeten Musik mal ganz nett.
+- Für einen weiteren Ausbau des Spiels wäre eine Funktion die ich befürworten würde die Einführung von verschiedenen Wachen-Größe bzw Wachen mit unterschiedlich großen Sicht-Bereichen.
+-Wenn Space zum Starten verwendet wird, dann auch Space zum nächsten Level benutzen, um einen Flow in die Tasten-Kombination zu bekommen.  Und im Umkehrschluss dann Enter zum wiederholen des Levels.
+-Zum bestimmen der Richtung würde Ich Q/E präferieren, da sich diese  Tasten bei der WASD-Steuerung leichter erreichen lassen und bereits öfters in anderen Spielen zum drehen verwendet werden.
+-Die Tipps an der Seite vlt in einen rahmen Setzten oder irgendwie anders abtrennen, sodass es nicht einfach frei-stehende Schrift ist. Zudem beginnt die Schrift zwar auf der Mitte des Bildschirms, ist dann allerdings bei mehreren Tipps nicht mehr mittig.
+-Wenn man einen Gaurd ins Ziel zieht/schiebt gewinnt man auch direkt, was keinerlei Sinn ergibt. Das Ziel sollte nur ohne Guard funktionieren.
+-In den doch länger werdenden Anleitungen am Anfang eines Levels wäre etwas Farbe oder herausheben zur schnelleren Orientierung hilfreich. Zum Beispiel für die Tasten eine bestimmte Farbe oder Umrandungen.
+Ansonsten funktioniert das Spiel, zumindest bei mir Fehlerfrei und hat auch keine Probleme bei der Installation gehabt. In dem Genre geht es weniger um Grafik, als mehr um Rätsel zum lösen, deswegen sind meine Anmerkungen im Bezug auf Aussehen auch nur subjektive Wünsche, die ich für besser halten würde. Generell hält sich das Spiel in Sachen Schwierigkeitsgrad im einfachen Bereich, was ich allerdings für die ersten paar Level, welche auch als Tutorial für die Funktionen gelten, auch richtig finde. Sollten dann noch später Level hinzukommen würde das erhöhen des Schwierigkeitsgrad jedoch sicherlich von Nöten sein.
+Zudem lässt sich erkennen, dass Sie wohl beim erstellen der Level an diese Kästchen Struktur gebunden sind, was zwar am Anfang kein Problem darstellen sollte, jedoch im Späteren Verlauf eine Einschränkung darstellen könnte. Sollte allerdings die Anzahl dieser Kästchen bzw. die Größe des „Spielbretts" erweiterbar sein, so sehe ich auch darin kein Problem.
+Abschließend würde Ich sagen, dass das Spiel in seiner Grundfunktion auf jeden Fall funktioniert und nun nur noch das Ansprechende für den Spieler ausgebaut werden kann.</t>
+  </si>
+  <si>
+    <t>Arne Kaleck</t>
   </si>
 </sst>
 </file>
@@ -205,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -220,6 +325,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -536,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,8 +656,8 @@
     <col min="2" max="2" width="37.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" style="5" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
@@ -576,7 +684,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>42951</v>
       </c>
@@ -613,7 +721,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>25</v>
       </c>
@@ -670,7 +778,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>27</v>
@@ -790,7 +898,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>42991</v>
       </c>
@@ -810,7 +918,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>42993</v>
       </c>
@@ -824,10 +932,10 @@
         <v>5</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>44</v>
       </c>
@@ -836,6 +944,110 @@
       </c>
       <c r="D16" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>42994</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Übersicht über Testspiele aktualisiert
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
   <si>
     <t>Datum</t>
   </si>
@@ -245,9 +245,6 @@
     <t>Marcus Riemer</t>
   </si>
   <si>
-    <t>Erweiterungsvorschläge: mehr Level, bessers Interface, Schalter für Sound (anstatt Stein), Nachtlevel, Beleuchtung</t>
-  </si>
-  <si>
     <t>-Gute Funktion mit dem ablenken durch das werfen von Steinen, jedoch würde ich es besser finden, wenn die Guards dann nicht alle auf exakt die Selbe Position laufen, sondern maximal in die selber Ecke oder die Blickrichtung ändern.
 - Ich würde einen größeren Kontrast in die Farbwahl bringen. Generell sind viele Blau-Töne vertreten. Eventuell könnte man zum Beispiel realistische Farben nehmen. Beispielsweise Beige für Bürogebäude oder Stahl-Grau für „Agency-Gebäude".
 -Die Wände würde ich nicht nur mit einem Muster Kennzeichen, sondern eher In kompletter unterschiedlicher Farbe machen (hilft dann auch direkt beim Punkto monotone Farbwahl).
@@ -267,6 +264,27 @@
   </si>
   <si>
     <t>Arne Kaleck</t>
+  </si>
+  <si>
+    <t>Drehen der Wachen verbessern (erst stoppen, dann drehen, dann weiterlaufen, etc.); Erweiterungsvorschläge: mehr Level, bessers Interface, Schalter für Sound (anstatt Stein), Nachtlevel mit eingeschränktem Sichtradius des Spielers, Beleuchtung</t>
+  </si>
+  <si>
+    <t>Jan Helke</t>
+  </si>
+  <si>
+    <t>Spielidee: Ich finde, das Spielprinzip „Vermeide die Sichtlinie der Gegner“ ist jetzt nicht sonderlich originell, da gab es in der Vergangenheit viele Titel, die entweder exakt das als Spielziel hatten oder bei denen diese Taktik mindestens hilfreich ist. Namen, die mir da einfallen sind „Splinter Cell“ und „Commandos – Hinter feindlichen Linien“. Aber: Ich ma das Spielprinzip, deshalb hatte ich Spaß beim Test.
+Hintergrund: Ich würde mir wünsche, einen minimalen Hintergrund zu haben. Irgendein einleitender Text „Du bist Spion und willst die DA ausspionieren. Pass auf, dass du dabei nicht erwischt wirst.“ Einfach, damit man nicht alleine mit dem Start-Button da sitzt und nicht weiß, was man machen muss.
+Schwierigkeit: Generell fand ich die Level alle recht einfach. Die Wachen wirken ziemlich statisch.
+Idee: Kann man den Wachen ein generelles Pattern geben, dass sie (egal, ob sie stillstehen oder sich bewegen) immer „den Kopf“ um 5 – 10 Grad in beide Richtungen drehen. Gerne auch in einem immer zufälligen Winkel. So wie jeder Mensch ja mal mehr mal weniger nach links oder rechts guckt. Ich könnte mir vorstellen, dass das als generische Funktion aller Wachen recht einfach einzubauen sein müsste.
+Level 1: Die obere Wache sollte sich beim Wenden in den Raum hinein drehen. Es ist unwahrscheinlich, dass sie beim Drehen immer die Wand angucken würde.
+Level 2: Ich finde die obere Wache ziemlich dämlich. Die sollte sich auf jeden Fall beständig langsam von links nach rechts und zurück drehen. Kann man die Disquise-Option ausblenden? Die braucht man hier noch nicht und sie ist nicht erklärt.
+Level 3: Auch hier würde ich die Disquise Option ausblenden. Ich würde ansonsten auch die Benutzung der Shift Taste ändern. Und zwar würde ich das „Wache durch die Gegend schleifen“ nur machen, wenn die Taste gedrückt gehalten wird. Das fühlt sich einfach haptisch besser an, dass ich die Taste halten muss, während ich die Wache ziehe. Wie beim Laufen, da muss ich ja auch Halten. Und sobald ich die Taste loslasse, lass ich die Wache exakt da liegen, wo sie liegt.
+Level 4: In dem Level ist mir das mit den stur nach vorne schauenden Wachen besonders aufgefallen. Es würde lebendiger wirken, wenn sie ein bisschen schwenken würden. Das hätte zwar keine Auswirkungen auf die Schwierigkeit des Levels, wirkt aber aktiver. Ansonsten habe ich festgestellt, dass sich der schwarze Ring um den Chrakter anders verhält. Im normalen Modus ist der so etwas wie eine Pufferzone. Wenn der schwarze Ring in den Sichtbereich einer Wache gerät, passiert erst mal gar nichts. Der Alarm geht erst los, wenn die Wache den inneren Ring „sieht“. Wenn der Charakter getarnt ist, werden die Wachen getriggert in dem Moment, wenn sie den schwarzen Ring sehen. Das würde ich vereinheitlichen und den schwarzen Ring bei beiden Varianten als Pufferzone nutzen.
+Level 5: Im Text steht zwar, dass man die Wurfweite ändern kann, je nachdem, wie lange man die Taste hält. Ich würde aber noch einen Hinweis auf die farbliche Veränderung des Steins je nach Wurfkraft einbauen.
+Level 6: Gefällt mir gut. Es kommen unterschiedliche Elemente zum Einsatz und es gibt verschiedene Arten, das Level zu lösen. Ich würde der oberen Wache einen etwas komplizierteren Weg geben. Und zwar dass sie sich an der rechten unteren Ecke ihres Weges umdreht und dann den Weg in die entgegengesetzte Richtung geht. Das zeigt auch, dass die Wachen etwas mehr können als nur im Krei zu laufen.</t>
+  </si>
+  <si>
+    <t>Lars' Bruder</t>
   </si>
 </sst>
 </file>
@@ -644,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +811,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>42985</v>
       </c>
@@ -813,7 +831,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>42986</v>
       </c>
@@ -850,7 +868,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>42987</v>
       </c>
@@ -867,7 +885,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>42988</v>
       </c>
@@ -881,7 +899,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>42990</v>
       </c>
@@ -918,7 +936,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>42993</v>
       </c>
@@ -949,7 +967,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>42994</v>
       </c>
@@ -1022,7 +1040,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>45</v>
       </c>
@@ -1033,7 +1051,7 @@
         <v>55</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
@@ -1044,10 +1062,35 @@
         <v>4</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first Bug Fixes after Testing
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t>Datum</t>
   </si>
@@ -285,6 +285,12 @@
   </si>
   <si>
     <t>Lars' Bruder</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_22.exe</t>
+  </si>
+  <si>
+    <t>Wachen können im Jagdmodus nicht mehr zwischendrin in den Suchmodus wechseln; Wachen berechnen im Patrol- und Suchmodus nur noch 1x den Weg (im Jagdmodus alle 0.5 Sekunden, aber manuell neuen Path anfordern, sie haben sich sonst manchmal aufgehängt); Component für Pathfinding wird, wenn möglich, komplett deaktiviert (anstatt nur Berechnungen deaktiviert); Erreichen des Ziels von Wachen (auch toter, die geschoben werden) führt nicht mehr zum Gewinnen; Tastaturbefehle werden jetzt immer erkannt, auch wenn Grafikeinstellungen auf "Niedrigst" sind (insb. auch Loslassen der Shift-Taste) (von FixedUpdate zu Update verschoben); Werfen des Steins ruft Wachen zur tatsächlich getroffenen Position (z.B. Wand, die getroffen wird), anstatt zur errechneten maximalen Poition gemäß Wurfreichweite</t>
   </si>
 </sst>
 </file>
@@ -662,10 +668,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,6 +1100,23 @@
         <v>61</v>
       </c>
     </row>
+    <row r="26" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>43000</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tutorial Levels have deactivated functions etc.
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
   <si>
     <t>Datum</t>
   </si>
@@ -290,7 +290,13 @@
     <t>DiscordiaAgency_Demo_2017_09_22.exe</t>
   </si>
   <si>
-    <t>Wachen können im Jagdmodus nicht mehr zwischendrin in den Suchmodus wechseln; Wachen berechnen im Patrol- und Suchmodus nur noch 1x den Weg (im Jagdmodus alle 0.5 Sekunden, aber manuell neuen Path anfordern, sie haben sich sonst manchmal aufgehängt); Component für Pathfinding wird, wenn möglich, komplett deaktiviert (anstatt nur Berechnungen deaktiviert); Erreichen des Ziels von Wachen (auch toter, die geschoben werden) führt nicht mehr zum Gewinnen; Tastaturbefehle werden jetzt immer erkannt, auch wenn Grafikeinstellungen auf "Niedrigst" sind (insb. auch Loslassen der Shift-Taste) (von FixedUpdate zu Update verschoben); Werfen des Steins ruft Wachen zur tatsächlich getroffenen Position (z.B. Wand, die getroffen wird), anstatt zur errechneten maximalen Poition gemäß Wurfreichweite</t>
+    <t>Wachen können im Jagdmodus nicht mehr zwischendrin in den Suchmodus wechseln; Wachen berechnen im Patrol- und Suchmodus nur noch 1x den Weg (im Jagdmodus pro Frame manuell neuen Path anfordern); Component für Pathfinding wird nicht komplett deaktiviert (sonst Error, wenn Seeker noch aktiv, stattdessen nur canMove auf false setzen); Erreichen des Ziels von Wachen (auch toter, die geschoben werden) führt nicht mehr zum Gewinnen; Tastaturbefehle werden jetzt immer erkannt, auch wenn Grafikeinstellungen auf "Niedrigst" sind (insb. auch Loslassen der Shift-Taste) (von FixedUpdate zu Update verschoben); Werfen des Steins ruft Wachen zur tatsächlich getroffenen Position (z.B. Wand, die getroffen wird), anstatt zur errechneten maximalen Poition gemäß Wurfreichweite; tote Wachen können nicht mehr alerted werden oder den Spieler jagen</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_22-2.exe</t>
+  </si>
+  <si>
+    <t>Kugeln spawnen korrekt aus den Pistolen der Wachen anstatt aus Wachen-Mittelpunkt; Tutorial-Levels haben nur Features aktiviert, die auch benutzt werden sollen; SPACE führt jetzt immer weiter/zum nächsten Level, ENTER ist dazu da, das aktuelle Level (sofern gewonnen) zu wiederholen</t>
   </si>
 </sst>
 </file>
@@ -668,11 +674,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,7 +1106,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="255" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>43000</v>
       </c>
@@ -1115,6 +1121,20 @@
       </c>
       <c r="E26" s="5" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can walk over dead Guards now
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -296,7 +296,7 @@
     <t>DiscordiaAgency_Demo_2017_09_22-2.exe</t>
   </si>
   <si>
-    <t>Kugeln spawnen korrekt aus den Pistolen der Wachen anstatt aus Wachen-Mittelpunkt; Tutorial-Levels haben nur Features aktiviert, die auch benutzt werden sollen; SPACE führt jetzt immer weiter/zum nächsten Level, ENTER ist dazu da, das aktuelle Level (sofern gewonnen) zu wiederholen</t>
+    <t>Kugeln spawnen korrekt aus den Pistolen der Wachen anstatt aus Wachen-Mittelpunkt; Tutorial-Levels haben nur Features aktiviert, die auch benutzt werden sollen; SPACE führt jetzt immer weiter/zum nächsten Level, ENTER ist dazu da, das aktuelle Level (sofern gewonnen) zu wiederholen; Kontrast des FOV ist besser; Spieler kann jetzt über tote Wachen rüberlaufen (Kollision mit Wänden funktioniert nachwievor)</t>
   </si>
 </sst>
 </file>
@@ -678,7 +678,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1123,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Impact Radius has animation!
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
   <si>
     <t>Datum</t>
   </si>
@@ -297,6 +297,12 @@
   </si>
   <si>
     <t>Kugeln spawnen korrekt aus den Pistolen der Wachen anstatt aus Wachen-Mittelpunkt; Tutorial-Levels haben nur Features aktiviert, die auch benutzt werden sollen; SPACE führt jetzt immer weiter/zum nächsten Level, ENTER ist dazu da, das aktuelle Level (sofern gewonnen) zu wiederholen; Kontrast des FOV ist besser; Spieler kann jetzt über tote Wachen rüberlaufen (Kollision mit Wänden funktioniert nachwievor); 2 neue Level; Smoothing beim Pathfinding; Cheat Keys, um zu bestimmten Level zu springen</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_22-3.exe</t>
+  </si>
+  <si>
+    <t>Animierter Impact-Radius für auftreffende Objekte; Audio-Radius nur noch 7.5 anstatt 10 Einheiten; Respawnen der Gegenstände dauert jetzt 10 Sekunden</t>
   </si>
 </sst>
 </file>
@@ -674,11 +680,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +694,7 @@
     <col min="3" max="3" width="14" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="69.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="114.85546875" style="5" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
@@ -715,7 +721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>42951</v>
       </c>
@@ -809,7 +815,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>27</v>
@@ -843,6 +849,9 @@
       <c r="F8" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -861,7 +870,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>42986</v>
       </c>
@@ -929,7 +938,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>42991</v>
       </c>
@@ -966,7 +975,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>44</v>
       </c>
@@ -978,6 +987,9 @@
       </c>
       <c r="F16" s="5" t="s">
         <v>47</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="150" x14ac:dyDescent="0.25">
@@ -1011,7 +1023,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1053,7 +1065,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>45</v>
       </c>
@@ -1135,6 +1147,20 @@
       </c>
       <c r="E27" s="5" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A lot of bugs fixed; Guards rotate now
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
   <si>
     <t>Datum</t>
   </si>
@@ -303,6 +303,28 @@
   </si>
   <si>
     <t>Animierter Impact-Radius für auftreffende Objekte; Audio-Radius nur noch 7.5 anstatt 10 Einheiten; Respawnen der Gegenstände dauert jetzt 10 Sekunden</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_23.exe</t>
+  </si>
+  <si>
+    <t>Intro-Text im Startmenü; Hilfe-Seite mit Steuerung; Wachen bleiben jetzt mit etwas Abstand zum aufgetroffenen Objekt</t>
+  </si>
+  <si>
+    <t>dragged Guard still collides with other dead Guards; speed-run-achievements and level timer; bullets still rather easy to avoid; Level 7: very easy, more guards, or 2 guards on same path; guards they should say "hello" or "yo dawg" when meeting each other; try Deus Ex &amp; Commandos 2 as inspiration; "why are you always going towards the exit?" -&gt; Target Sprite needs to be changed, probably, or use them as exits and chain levels, so you need to go through several rooms, before actually seeing an assassination target that you have to specifically kill somehow; maybe have "strong" guards that cannot be disabled; or cameras, that can't shoot you, but alert some guards to you; [12:50] [Group] [Anuschka]: btw. are the level intro fonts still too large for your screen?
+[12:50] [Group] [*Pel]: hmm it's better at least
+[12:51] [Group] [*Pel]: and when guards yell "argh" it should alert nearby guards in a small radius :p
+[12:51] [Group] [*Pel]: but that would affec t your level design
+[12:51] [Group] [*Pel]: they do yell quite loud...; [12:59] [Group] [*Pel]: and a narrator like in stanley's parable
+[12:59] [Group] [Anuschka]: lol
+[13:00] [Group] [*Pel]: "[player] hit the poor guard John on the back and is now struggling with his moral conscience"
+[13:00] [Group] [*Pel]: "does that make him a bad guy"</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_23-2.exe</t>
+  </si>
+  <si>
+    <t>Tote Wachen können nicht mehr miteinander kollidieren; Bug: angezeigter Radius der Geräuschquelle stimmt nicht mit Hörweite überein; Bug: falsche Ausgangsposition für Rufradius der Wachen; Wachen rotieren leicht nach links und rechts, nachdem sie Geräusch gefolgt sind; stationäre Wachen rotieren leicht nach links und rechts</t>
   </si>
 </sst>
 </file>
@@ -680,11 +702,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,6 +1185,51 @@
         <v>67</v>
       </c>
     </row>
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>43001</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FOV is fixed to be accurate now.
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="75">
   <si>
     <t>Datum</t>
   </si>
@@ -325,6 +325,12 @@
   </si>
   <si>
     <t>Tote Wachen können nicht mehr miteinander kollidieren; Bug: angezeigter Radius der Geräuschquelle stimmt nicht mit Hörweite überein; Bug: falsche Ausgangsposition für Rufradius der Wachen; Wachen rotieren leicht nach links und rechts, nachdem sie Geräusch gefolgt sind; stationäre Wachen rotieren leicht nach links und rechts</t>
+  </si>
+  <si>
+    <t>Wachen-Sichtradius schlägt jetzt auch schon an, wenn man seitlich rein kommt, d.h. wenn noch nicht Mittelpunkt des Spielers oder toten Körpers drin ist</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_23-3.exe</t>
   </si>
 </sst>
 </file>
@@ -702,11 +708,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,6 +1236,20 @@
         <v>72</v>
       </c>
     </row>
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New Controls, Player less drag
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="77">
   <si>
     <t>Datum</t>
   </si>
@@ -331,6 +331,12 @@
   </si>
   <si>
     <t>DiscordiaAgency_Demo_2017_09_23-3.exe</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_23-4.exe</t>
+  </si>
+  <si>
+    <t>neue Steuerung; Spieler jetzt mit noch weniger Drag</t>
   </si>
 </sst>
 </file>
@@ -708,11 +714,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,6 +1256,20 @@
         <v>73</v>
       </c>
     </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Level 7-8 harder. Bug fixes according to Excel sheet.
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="79">
   <si>
     <t>Datum</t>
   </si>
@@ -337,6 +337,12 @@
   </si>
   <si>
     <t>neue Steuerung; Spieler jetzt mit noch weniger Drag</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_24.exe</t>
+  </si>
+  <si>
+    <t>Hauptmenü: keine Fehlermeldung mehr, dass Objekt nicht gefunden; Hauptmenü: Musik startet nicht mehr erneut, wenn zur Steuerungsübersicht gewechselt wird; zufälliges Rotieren der Wachen funktioniert jetzt auch um 0 Grad herum; Level 7 und 8 schwerer gemacht; Verkleiden klappt, auch wenn man über 2 toten Körpern steht</t>
   </si>
 </sst>
 </file>
@@ -714,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -1270,6 +1276,20 @@
         <v>76</v>
       </c>
     </row>
+    <row r="34" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added some Menu Buttons
</commit_message>
<xml_diff>
--- a/Development_Testing/Übersicht.xlsx
+++ b/Development_Testing/Übersicht.xlsx
@@ -13,7 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Balancing" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Balancing!$G$1:$I$4</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="102">
   <si>
     <t>Datum</t>
   </si>
@@ -344,12 +348,84 @@
   <si>
     <t>Hauptmenü: keine Fehlermeldung mehr, dass Objekt nicht gefunden; Hauptmenü: Musik startet nicht mehr erneut, wenn zur Steuerungsübersicht gewechselt wird; zufälliges Rotieren der Wachen funktioniert jetzt auch um 0 Grad herum; Level 7 und 8 schwerer gemacht; Verkleiden klappt, auch wenn man über 2 toten Körpern steht</t>
   </si>
+  <si>
+    <t>Wachen</t>
+  </si>
+  <si>
+    <t>Auftragskiller</t>
+  </si>
+  <si>
+    <t>Such-Modus</t>
+  </si>
+  <si>
+    <t>Jagd-Modus</t>
+  </si>
+  <si>
+    <t>Patroullien-Modus</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Aufmerksam</t>
+  </si>
+  <si>
+    <t>Sichtradius</t>
+  </si>
+  <si>
+    <t>Sichtwinkel</t>
+  </si>
+  <si>
+    <t>Verkleidet</t>
+  </si>
+  <si>
+    <t>60°</t>
+  </si>
+  <si>
+    <t>2.0f</t>
+  </si>
+  <si>
+    <t>x0.5</t>
+  </si>
+  <si>
+    <t>x2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lauf-
+geschwindigkeit </t>
+  </si>
+  <si>
+    <t>Rotations-
+geschwindigkeit</t>
+  </si>
+  <si>
+    <t>x1.5</t>
+  </si>
+  <si>
+    <t>1.0f</t>
+  </si>
+  <si>
+    <t>3.0f</t>
+  </si>
+  <si>
+    <t>x1.0</t>
+  </si>
+  <si>
+    <t>x2.0 (eingestellt)
+x1.6 (gemessen)</t>
+  </si>
+  <si>
+    <t>DiscordiaAgency_Demo_2017_09_25.exe</t>
+  </si>
+  <si>
+    <t>Platzhalter-Buttons auf Startmenü eingeführt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,6 +440,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -386,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -405,6 +496,35 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -720,11 +840,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,7 +1410,149 @@
         <v>78</v>
       </c>
     </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09AFC6CC-FF9E-41B2-98ED-C851EEFC13DE}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="20" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="7"/>
+    <col min="6" max="6" width="2.7109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13" style="7" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>